<commit_message>
Fix <Afficher les totaux des montants> issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -400,13 +400,13 @@
         <v>Périodicité</v>
       </c>
       <c r="G1" t="str">
+        <v>Taux de taxe</v>
+      </c>
+      <c r="H1" t="str">
         <v>MT brut de loyer</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>MT brut d'avance</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Taux de taxe</v>
       </c>
       <c r="J1" t="str">
         <v>Taxe/loyer</v>
@@ -441,10 +441,10 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>5000</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -482,10 +482,10 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>5000</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -522,14 +522,14 @@
       <c r="F4" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
         <v>--</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>15000</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -564,13 +564,13 @@
         <v>trimestrielle</v>
       </c>
       <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>28000</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>2800</v>
@@ -605,10 +605,10 @@
         <v>trimestrielle</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>12000</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -646,10 +646,10 @@
         <v>mensuelle</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>9000</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -687,13 +687,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
         <v>6000</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>600</v>
@@ -728,13 +728,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
         <v>6000</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>600</v>
@@ -769,13 +769,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
         <v>14000</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>2100</v>
@@ -810,10 +810,10 @@
         <v>mensuelle</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>5000</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -851,13 +851,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
         <v>5000</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>500</v>
@@ -891,14 +891,14 @@
       <c r="F13" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G13" t="str">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="str">
         <v>--</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>10000</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -932,14 +932,14 @@
       <c r="F14" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="str">
         <v>--</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>10000</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -974,13 +974,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15">
         <v>24000</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>3600</v>
@@ -1015,13 +1015,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
         <v>36000</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>5400</v>
@@ -1056,13 +1056,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
         <v>40000</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>6000</v>
@@ -1097,13 +1097,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18">
         <v>30000</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>4500</v>
@@ -1138,13 +1138,13 @@
         <v>mensuelle</v>
       </c>
       <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19">
         <v>12000</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>1800</v>
@@ -1159,9 +1159,50 @@
         <v>10200</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G20" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H20">
+        <v>237000</v>
+      </c>
+      <c r="I20">
+        <v>35000</v>
+      </c>
+      <c r="J20">
+        <v>27900</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>90000</v>
+      </c>
+      <c r="M20">
+        <v>244100</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change calcul to <arrondie> in situation de cloture
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>910/TANGER /AV1</v>
+        <v>949/DR</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>D235689</v>
+        <v>BG12456</v>
       </c>
       <c r="D2" t="str">
-        <v>KAMILIA LALA</v>
+        <v>HAYLALA ONE</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -441,39 +441,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>24000</v>
+        <v>4334.4</v>
       </c>
       <c r="I2">
-        <v>24000</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>3600</v>
+        <v>433.44</v>
       </c>
       <c r="K2">
-        <v>3600</v>
-      </c>
-      <c r="L2" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>20400</v>
+        <v>3900.96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>910/TANGER /AV1</v>
+        <v>949/DR</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>K3544354</v>
+        <v>BG196435</v>
       </c>
       <c r="D3" t="str">
-        <v>ABDOU FAFA</v>
+        <v>HAYLAL TWO</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,80 +482,80 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>13354.4</v>
+        <v>5665.73</v>
       </c>
       <c r="I3">
-        <v>13354.4</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>2003.16</v>
+        <v>566.57</v>
       </c>
       <c r="K3">
-        <v>2003.16</v>
-      </c>
-      <c r="L3" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>11351.24</v>
+        <v>5099.16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>910/TANGER /AV1</v>
+        <v>001/LF/TEST DR/AV1</v>
       </c>
       <c r="B4" t="str">
-        <v>Direction régionale</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C4" t="str">
-        <v>L254654</v>
+        <v>11986345</v>
       </c>
       <c r="D4" t="str">
-        <v>SAMIR DADA</v>
+        <v>ALI EXPRESSE</v>
       </c>
       <c r="E4" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F4" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>2645.6</v>
+        <v>30000</v>
       </c>
       <c r="I4">
-        <v>2645.6</v>
+        <v>30000</v>
       </c>
       <c r="J4">
-        <v>264.56</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>264.56</v>
+        <v>0</v>
       </c>
       <c r="L4" t="str">
         <v>--</v>
       </c>
       <c r="M4">
-        <v>2381.04</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>115/TANGER MED/AV1</v>
+        <v>001/TEST DR</v>
       </c>
       <c r="B5" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>L5245475</v>
+        <v>BG432432</v>
       </c>
       <c r="D5" t="str">
-        <v>MORAD JOJO</v>
+        <v>TETS TESTS</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -564,153 +564,71 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>9000</v>
+        <v>20000</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="J5">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="L5" t="str">
         <v>--</v>
       </c>
       <c r="M5">
-        <v>8100</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>115/TANGER MED/AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B6" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C6" t="str">
-        <v>Z213568</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D6" t="str">
-        <v>NABIL MOMO</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E6" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G6" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H6">
-        <v>6000</v>
+        <v>60000.13</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>600</v>
+        <v>4000.01</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" t="str">
-        <v>--</v>
+      <c r="L6">
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>115/TANGER MED/AV1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C7" t="str">
-        <v>L525655</v>
-      </c>
-      <c r="D7" t="str">
-        <v>KHALID RARA</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>6000</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>600</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="str">
-        <v>--</v>
-      </c>
-      <c r="M7">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H8">
-        <v>61000</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>7967.72</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>53032.28</v>
+        <v>56000.12</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Regroup deplucated proprietaire in <annex 1>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,7 +423,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>949/DR</v>
+        <v>049/DR 2</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
@@ -438,42 +438,42 @@
         <v>non</v>
       </c>
       <c r="F2" t="str">
-        <v>mensuelle</v>
+        <v>annuelle</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2">
-        <v>4334.4</v>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>433.44</v>
+        <v>100000</v>
+      </c>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="M2">
-        <v>3900.96</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>949/DR</v>
+        <v>094/DR 1</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>BG196435</v>
+        <v>BG12456</v>
       </c>
       <c r="D3" t="str">
-        <v>HAYLAL TWO</v>
+        <v>HAYLALA ONE</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,80 +482,80 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>5665.73</v>
+        <v>15</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>566.57</v>
+        <v>10000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M3">
-        <v>5099.16</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>001/LF/TEST DR/AV1</v>
+        <v>949/DR</v>
       </c>
       <c r="B4" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>11986345</v>
+        <v>BG12456</v>
       </c>
       <c r="D4" t="str">
-        <v>ALI EXPRESSE</v>
+        <v>HAYLALA ONE</v>
       </c>
       <c r="E4" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F4" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>30000</v>
+        <v>4334.4</v>
       </c>
       <c r="I4">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>433.44</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" t="str">
-        <v>--</v>
+      <c r="L4">
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>30000</v>
+        <v>3900.96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>001/TEST DR</v>
+        <v>949/DR</v>
       </c>
       <c r="B5" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>BG432432</v>
+        <v>BG196435</v>
       </c>
       <c r="D5" t="str">
-        <v>TETS TESTS</v>
+        <v>HAYLAL TWO</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -564,71 +564,153 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>20000</v>
+        <v>5665.73</v>
       </c>
       <c r="I5">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>3000</v>
+        <v>566.57</v>
       </c>
       <c r="K5">
-        <v>3000</v>
-      </c>
-      <c r="L5" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>17000</v>
+        <v>5099.16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>001/LF/TEST DR/AV1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C6" t="str">
+        <v>11986345</v>
+      </c>
+      <c r="D6" t="str">
+        <v>ALI EXPRESSE</v>
+      </c>
+      <c r="E6" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>30000</v>
+      </c>
+      <c r="I6">
+        <v>30000</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="str">
+        <v>--</v>
+      </c>
+      <c r="M6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>001/TEST DR</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C7" t="str">
+        <v>BG432432</v>
+      </c>
+      <c r="D7" t="str">
+        <v>TETS TESTS</v>
+      </c>
+      <c r="E7" t="str">
+        <v>non</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>20000</v>
+      </c>
+      <c r="I7">
+        <v>20000</v>
+      </c>
+      <c r="J7">
+        <v>3000</v>
+      </c>
+      <c r="K7">
+        <v>3000</v>
+      </c>
+      <c r="L7" t="str">
+        <v>--</v>
+      </c>
+      <c r="M7">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B6" t="str">
+      <c r="B8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C6" t="str">
+      <c r="C8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D6" t="str">
+      <c r="D8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E6" t="str">
+      <c r="E8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F6" t="str">
+      <c r="F8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G6" t="str">
+      <c r="G8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H6">
+      <c r="H8">
         <v>60000.13</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
+      <c r="I8">
+        <v>110000</v>
+      </c>
+      <c r="J8">
         <v>4000.01</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>56000.12</v>
+      <c r="K8">
+        <v>11500</v>
+      </c>
+      <c r="L8">
+        <v>110000</v>
+      </c>
+      <c r="M8">
+        <v>264500.12</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>